<commit_message>
Teensy Arbotix Pro - Update parts list
</commit_message>
<xml_diff>
--- a/Teensy Arbotix Pro/Teesny Arbotix Pro BOM.xlsx
+++ b/Teensy Arbotix Pro/Teesny Arbotix Pro BOM.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BOM" localSheetId="0">Sheet1!$B$1:$G$27</definedName>
+    <definedName name="BOM" localSheetId="0">Sheet1!$B$1:$G$24</definedName>
   </definedNames>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -103,24 +103,6 @@
     <t>C2, C3, C9</t>
   </si>
   <si>
-    <t>1x8 Connector</t>
-  </si>
-  <si>
-    <t>HDR-1x8</t>
-  </si>
-  <si>
-    <t>CN1S, CN2S, JD0-7</t>
-  </si>
-  <si>
-    <t>2x8 Connector</t>
-  </si>
-  <si>
-    <t>HDR-2x8</t>
-  </si>
-  <si>
-    <t>CN2P</t>
-  </si>
-  <si>
     <t>POWER_JACKPTH</t>
   </si>
   <si>
@@ -130,24 +112,6 @@
     <t>J1</t>
   </si>
   <si>
-    <t>1x4 Connector</t>
-  </si>
-  <si>
-    <t>HDR-1x4</t>
-  </si>
-  <si>
-    <t>J2, J5V, JGND</t>
-  </si>
-  <si>
-    <t>1x3 Connector</t>
-  </si>
-  <si>
-    <t>HDR-1x3</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
     <t>WM18887-ND</t>
   </si>
   <si>
@@ -157,15 +121,6 @@
     <t>JAX1, JAX2, JAX3, JAX4, JAX5, JAX-PWR</t>
   </si>
   <si>
-    <t>1x6 Connector</t>
-  </si>
-  <si>
-    <t>HDR-1x6</t>
-  </si>
-  <si>
-    <t>JD8-13</t>
-  </si>
-  <si>
     <t>Sparkfun LSM9DS1</t>
   </si>
   <si>
@@ -308,14 +263,61 @@
   </si>
   <si>
     <t>311-120CRCT-ND</t>
+  </si>
+  <si>
+    <t>2x7 connector - bottom teensy</t>
+  </si>
+  <si>
+    <t>SAM8882-ND</t>
+  </si>
+  <si>
+    <t>Digi-key Part numbers</t>
+  </si>
+  <si>
+    <t>102-1155-ND</t>
+  </si>
+  <si>
+    <t>A26508-40-ND</t>
+  </si>
+  <si>
+    <t>CONN HDR BRKWAY .100 40POS VERT</t>
+  </si>
+  <si>
+    <t>95?</t>
+  </si>
+  <si>
+    <t>A34268-40-ND</t>
+  </si>
+  <si>
+    <t>CONN HDR BRKWAY .100 80POS VERT</t>
+  </si>
+  <si>
+    <t>1x40 breakaway</t>
+  </si>
+  <si>
+    <t>2x40 breakaway</t>
+  </si>
+  <si>
+    <t>1276-2742-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 160-1405-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -358,13 +360,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -650,16 +659,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" style="5" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
@@ -667,29 +676,32 @@
     <col min="7" max="7" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>76</v>
+      <c r="A2" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -725,6 +737,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -745,8 +760,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>77</v>
+      <c r="A5" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -768,425 +783,384 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>20</v>
-      </c>
-      <c r="F6">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
       </c>
       <c r="F8">
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>32</v>
       </c>
-      <c r="F10">
+      <c r="F12">
         <v>3</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>35</v>
       </c>
-      <c r="F11">
+      <c r="F13">
         <v>3</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
         <v>37</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
         <v>38</v>
       </c>
-      <c r="F12">
-        <v>6</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
         <v>40</v>
       </c>
-      <c r="F13">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
         <v>42</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
         <v>44</v>
       </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
         <v>47</v>
       </c>
-      <c r="F15">
-        <v>3</v>
-      </c>
-      <c r="G15" t="s">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
         <v>49</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
         <v>50</v>
       </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>120</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
         <v>52</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="F17">
-        <v>3</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
         <v>55</v>
       </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
         <v>56</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
         <v>58</v>
       </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19">
-        <v>2</v>
-      </c>
-      <c r="G19" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23">
+        <v>47</v>
+      </c>
+      <c r="G23" t="s">
         <v>60</v>
       </c>
-      <c r="C20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="G21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="G22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23">
-        <v>120</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
-        <v>69</v>
-      </c>
       <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
-      </c>
-      <c r="G25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26">
-        <v>47</v>
-      </c>
-      <c r="G26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D27">
-        <v>42</v>
-      </c>
-      <c r="F27">
-        <v>150</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Parts list for V0.2
</commit_message>
<xml_diff>
--- a/Teensy Arbotix Pro/Teesny Arbotix Pro BOM.xlsx
+++ b/Teensy Arbotix Pro/Teesny Arbotix Pro BOM.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BOM" localSheetId="0">Sheet1!$B$1:$G$24</definedName>
+    <definedName name="BOM" localSheetId="0">Sheet1!$B$1:$G$29</definedName>
   </definedNames>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="121">
   <si>
     <t>Name</t>
   </si>
@@ -172,15 +172,9 @@
     <t>40K</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
-    <t>R2, R7, R8, R11, R13</t>
-  </si>
-  <si>
     <t>RES_0402</t>
   </si>
   <si>
@@ -193,9 +187,6 @@
     <t>1K</t>
   </si>
   <si>
-    <t>R5</t>
-  </si>
-  <si>
     <t>4.7K</t>
   </si>
   <si>
@@ -302,13 +293,167 @@
   </si>
   <si>
     <t xml:space="preserve"> 160-1405-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMBT6428TR-ND
+</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>TRANSISTOR GP NPN AMP SOT-23</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>v0.1</t>
+  </si>
+  <si>
+    <t>v0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAV16WDICT-ND
+</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>SOD-123</t>
+  </si>
+  <si>
+    <t>DIODE SWITCH 75V 400MW SOD-123</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 32V</t>
+  </si>
+  <si>
+    <t>CKN10244DKR-ND</t>
+  </si>
+  <si>
+    <t>S1, S2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">399-1168-1-ND
+</t>
+  </si>
+  <si>
+    <t>CAP_0805</t>
+  </si>
+  <si>
+    <t>C1, C4</t>
+  </si>
+  <si>
+    <t>v0.2 0 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">160-1427-1-ND
+</t>
+  </si>
+  <si>
+    <t>LED SUPER RED CLR THIN 0805 SMD</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>LED-0805</t>
+  </si>
+  <si>
+    <t>PWR, L2</t>
+  </si>
+  <si>
+    <t>311-51ARCT-ND</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>311-470ARCT-ND</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <r>
+      <t>R5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, R18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">R2, R7, R8, R11, R13, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R14, R15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> R16</t>
+    </r>
+  </si>
+  <si>
+    <t>NEO</t>
+  </si>
+  <si>
+    <t>Adafruit:: 1655</t>
+  </si>
+  <si>
+    <t>WS2812B 5050 RGB LED…</t>
+  </si>
+  <si>
+    <t>478-5230-1-ND</t>
+  </si>
+  <si>
+    <t>CAP TANT 10UF 16V 10% 1210</t>
+  </si>
+  <si>
+    <t>10uf</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>v0.2 - may play with different</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +465,27 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -342,9 +508,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -360,20 +524,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,26 +864,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32" style="5" customWidth="1"/>
+    <col min="1" max="1" width="32" style="14" customWidth="1"/>
     <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>75</v>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -692,16 +898,16 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>61</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -712,14 +918,14 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="8">
         <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -729,305 +935,320 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="8">
         <v>10</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="9">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="8">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="8">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="8">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="9">
+        <v>2</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="9">
+        <v>3</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="F15" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="8">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5">
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="8">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-      <c r="G13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="G17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
-      <c r="E16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="G17" t="s">
-        <v>47</v>
-      </c>
-    </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>71</v>
+      <c r="A18" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1035,128 +1256,314 @@
       <c r="E18" t="s">
         <v>40</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="8">
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>70</v>
+      <c r="A19" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="8">
         <v>2</v>
       </c>
       <c r="G19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="8">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="8">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="8">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>120</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="8">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="4">
+        <v>50</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="21">
+        <v>2</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="4">
+        <v>470</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="21">
+        <v>2</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20">
+      <c r="F26" s="8">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="8">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="8">
+        <v>47</v>
+      </c>
+      <c r="G28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="11">
+        <v>2</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="4">
+        <v>2</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="21"/>
+      <c r="G33" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H33" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="G21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22">
-        <v>5</v>
-      </c>
-      <c r="G22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23">
-        <v>47</v>
-      </c>
-      <c r="G23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>14</v>
+    </row>
+    <row r="34" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="4">
+        <v>2</v>
+      </c>
+      <c r="E34" s="4">
+        <v>1210</v>
+      </c>
+      <c r="F34" s="21"/>
+      <c r="G34" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Teensy Arbotix Pro: update parts list for version .2
</commit_message>
<xml_diff>
--- a/Teensy Arbotix Pro/Teesny Arbotix Pro BOM.xlsx
+++ b/Teensy Arbotix Pro/Teesny Arbotix Pro BOM.xlsx
@@ -223,13 +223,7 @@
     <t>811-3014-ND, 811-2692-ND</t>
   </si>
   <si>
-    <t>PCE3904DKR-ND</t>
-  </si>
-  <si>
     <t>CP-102A-ND</t>
-  </si>
-  <si>
-    <t>SUM110P04-05-E3DKR-ND</t>
   </si>
   <si>
     <t>BSS138CT-ND</t>
@@ -314,10 +308,6 @@
     <t>v0.2</t>
   </si>
   <si>
-    <t xml:space="preserve">BAV16WDICT-ND
-</t>
-  </si>
-  <si>
     <t>D5</t>
   </si>
   <si>
@@ -328,9 +318,6 @@
   </si>
   <si>
     <t>SWITCH TACTILE SPST-NO 0.05A 32V</t>
-  </si>
-  <si>
-    <t>CKN10244DKR-ND</t>
   </si>
   <si>
     <t>S1, S2</t>
@@ -447,6 +434,18 @@
   </si>
   <si>
     <t>v0.2 - may play with different</t>
+  </si>
+  <si>
+    <t>BAV16W-FDICT-ND</t>
+  </si>
+  <si>
+    <t>PCE3904CT-ND</t>
+  </si>
+  <si>
+    <t>CKN10244CT-ND</t>
+  </si>
+  <si>
+    <t>SUM110P04-05-E3CT-ND</t>
   </si>
 </sst>
 </file>
@@ -563,9 +562,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -578,6 +574,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -866,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +883,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -906,7 +905,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B2" t="s">
@@ -944,7 +943,7 @@
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>12</v>
@@ -965,15 +964,15 @@
         <v>14</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>13</v>
@@ -982,18 +981,18 @@
         <v>2</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>59</v>
+      <c r="A6" t="s">
+        <v>118</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -1016,38 +1015,38 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="B7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>78</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>60</v>
+      <c r="A9" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -1104,7 +1103,7 @@
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>27</v>
@@ -1125,38 +1124,38 @@
         <v>30</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="H13" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>31</v>
@@ -1174,35 +1173,35 @@
         <v>33</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="D15" s="4">
         <v>3</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>61</v>
+      <c r="A16" t="s">
+        <v>120</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
@@ -1221,8 +1220,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>62</v>
+      <c r="A17" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
@@ -1242,7 +1241,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
@@ -1260,12 +1259,12 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
@@ -1283,7 +1282,7 @@
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1308,7 +1307,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
@@ -1326,12 +1325,12 @@
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
@@ -1354,7 +1353,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
@@ -1377,7 +1376,7 @@
     </row>
     <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>40</v>
@@ -1391,16 +1390,16 @@
       <c r="E24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="20">
         <v>2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>40</v>
@@ -1414,16 +1413,16 @@
       <c r="E25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="20">
         <v>2</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
         <v>50</v>
@@ -1441,23 +1440,23 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="27" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="9">
         <v>5</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="6" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1480,10 +1479,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1493,67 +1492,67 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="D31" s="4">
         <v>1</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F31" s="11">
         <v>2</v>
       </c>
       <c r="G31" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="22" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>93</v>
       </c>
       <c r="D32" s="4">
         <v>2</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="20"/>
+      <c r="G33" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="D34" s="4">
         <v>2</v>
@@ -1561,9 +1560,9 @@
       <c r="E34" s="4">
         <v>1210</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="20"/>
       <c r="G34" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated parts list for Teensy Arbotix Pro
</commit_message>
<xml_diff>
--- a/Teensy Arbotix Pro/Teesny Arbotix Pro BOM.xlsx
+++ b/Teensy Arbotix Pro/Teesny Arbotix Pro BOM.xlsx
@@ -28,7 +28,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="BOM" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="1" name="BOM" type="6" refreshedVersion="5" deleted="1" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\Kurt\Documents\GitHub\Teensy3.1-Breakout-Boards\Teensy Arbotix Pro\BOM.csv" semicolon="1">
       <textFields count="6">
         <textField/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="131">
   <si>
     <t>Name</t>
   </si>
@@ -447,11 +447,41 @@
   <si>
     <t>SUM110P04-05-E3CT-ND</t>
   </si>
+  <si>
+    <t>ED8180-ND</t>
+  </si>
+  <si>
+    <t>CONN PIN SPRING-LOADED PCB GOLD</t>
+  </si>
+  <si>
+    <t>Reset pin maybe</t>
+  </si>
+  <si>
+    <t>296-38240-1-ND</t>
+  </si>
+  <si>
+    <t>IC BUFF/DVR TRI-ST DUAL 20SOIC</t>
+  </si>
+  <si>
+    <t>AX Buss 3.3 to 5v</t>
+  </si>
+  <si>
+    <t>296-37172-1-ND</t>
+  </si>
+  <si>
+    <t>IC BUFFER GATE SGL CMOS SOT23-5</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Neopixel 3.3 to 5v…</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -523,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -578,6 +608,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,6 +709,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -711,6 +761,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -863,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,6 +1632,64 @@
         <v>115</v>
       </c>
     </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>